<commit_message>
Quick edits made on the documents section of the project
</commit_message>
<xml_diff>
--- a/Documents/Documentation.xlsx
+++ b/Documents/Documentation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,6 +351,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -386,6 +403,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,7 +575,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>